<commit_message>
Gerrymon's Nautian Style - 3147664706 업데이트
</commit_message>
<xml_diff>
--- a/Data/Gerrymon's Nautian Style - 3147664706/3147664706.xlsx
+++ b/Data/Gerrymon's Nautian Style - 3147664706/3147664706.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\240122\Gerrymon's Nautian Style - 3147664706\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Gerrymon's Nautian Style - 3147664706\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5677394-94EE-49AA-87B7-0A480E2B6E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414D94EF-D34B-4B06-A7A2-B8A2317A58E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240203" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-03에 새로 추가된 노드들 (37개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{A4365D24-5CDE-4EC0-8E9B-C9A0AE207E4B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-03에 새로 추가된 노드들 (37개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="159">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -76,31 +112,446 @@
     <t>GM_Mer_Slab_Broad.description</t>
   </si>
   <si>
+    <t>StyleCategoryDef</t>
+  </si>
+  <si>
     <t>StyleCategoryDef+GM_Ocean.label</t>
   </si>
   <si>
-    <t>StyleCategoryDef</t>
-  </si>
-  <si>
     <t>GM_Ocean.label</t>
   </si>
   <si>
     <t>Nautian</t>
   </si>
   <si>
-    <t>노션</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>노션 석판 (대형)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>노션 석판 (중형)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>바닥을 장식하기 위한 해저 문명 양식의 석재 부조입니다.</t>
+    <t>DesignatorDropdownGroupDef+Ocean_Floor_FineTile.label</t>
+  </si>
+  <si>
+    <t>DesignatorDropdownGroupDef</t>
+  </si>
+  <si>
+    <t>Ocean_Floor_FineTile.label</t>
+  </si>
+  <si>
+    <t>Nautian fine tile</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Sandstone.description</t>
+  </si>
+  <si>
+    <t>TerrainDef</t>
+  </si>
+  <si>
+    <t>Exquisite stone tiles carved with Nautian style, made with no compromises, for expressing economic status. Slow to construct.</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Sandstone.label</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Sandstone.label</t>
+  </si>
+  <si>
+    <t>sandstone nautic fine tile</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Granite.description</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Granite.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Granite.label</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Granite.label</t>
+  </si>
+  <si>
+    <t>granite nautic fine tile</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Limestone.description</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Limestone.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Limestone.label</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Limestone.label</t>
+  </si>
+  <si>
+    <t>limestone nautic fine tile</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Slate.description</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Slate.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Slate.label</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Slate.label</t>
+  </si>
+  <si>
+    <t>slate nautic fine tile</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Marble.description</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Marble.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_Marble.label</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Marble.label</t>
+  </si>
+  <si>
+    <t>marble nautic fine tile</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_PristineLimeston.description</t>
+  </si>
+  <si>
+    <t>OceanFineTile_PristineLimeston.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanFineTile_PristineLimeston.label</t>
+  </si>
+  <si>
+    <t>OceanFineTile_PristineLimeston.label</t>
+  </si>
+  <si>
+    <t>pristine limestone nautic fine tile</t>
+  </si>
+  <si>
+    <t>DesignatorDropdownGroupDef+Ocean_Floor_OceanPavestone.label</t>
+  </si>
+  <si>
+    <t>Ocean_Floor_OceanPavestone.label</t>
+  </si>
+  <si>
+    <t>ocean stonefloor</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Sandstone.description</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Sandstone.description</t>
+  </si>
+  <si>
+    <t>Rough paved stone that mimic the ocean floor under the tide. These are not beautiful, but they make good surfaces for roads and outdoor walkways. Deconstructing flagstone yields no resources.</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Sandstone.label</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Sandstone.label</t>
+  </si>
+  <si>
+    <t>ocean sandstone floor</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Granite.description</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Granite.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Granite.label</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Granite.label</t>
+  </si>
+  <si>
+    <t>ocean granite floor</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Limestone.description</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Limestone.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Limestone.label</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Limestone.label</t>
+  </si>
+  <si>
+    <t>ocean limestone floor</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Slate.description</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Slate.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Slate.label</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Slate.label</t>
+  </si>
+  <si>
+    <t>ocean slate floor</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Marble.description</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Marble.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_Marble.label</t>
+  </si>
+  <si>
+    <t>OceanPavestone_Marble.label</t>
+  </si>
+  <si>
+    <t>ocean marble floor</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_PristineLimeston.description</t>
+  </si>
+  <si>
+    <t>OceanPavestone_PristineLimeston.description</t>
+  </si>
+  <si>
+    <t>TerrainDef+OceanPavestone_PristineLimeston.label</t>
+  </si>
+  <si>
+    <t>OceanPavestone_PristineLimeston.label</t>
+  </si>
+  <si>
+    <t>ocean pristine limestone floor</t>
+  </si>
+  <si>
+    <t>DesignatorDropdownGroupDef+Ocean_Floor_Carpet.label</t>
+  </si>
+  <si>
+    <t>Ocean_Floor_Carpet.label</t>
+  </si>
+  <si>
+    <t>nautic-style carpet</t>
+  </si>
+  <si>
+    <t>TerrainTemplateDef+Ocean_Floor_Seabed_Carpet.label</t>
+  </si>
+  <si>
+    <t>TerrainTemplateDef</t>
+  </si>
+  <si>
+    <t>Ocean_Floor_Seabed_Carpet.label</t>
+  </si>
+  <si>
+    <t>seabed carpet ({0})</t>
+  </si>
+  <si>
+    <t>TerrainTemplateDef+Ocean_Floor_Seabed_Carpet.description</t>
+  </si>
+  <si>
+    <t>Ocean_Floor_Seabed_Carpet.description</t>
+  </si>
+  <si>
+    <t>Soft carpet depicting the seabed under the wave. It's welcoming, cozy, and boosts the beauty of the room it's in. It's also quite flammable, and cleaning it is a laborious process</t>
+  </si>
+  <si>
+    <t>ThingDef+GM_Mer_ShellCurtain.label</t>
+  </si>
+  <si>
+    <t>GM_Mer_ShellCurtain.label</t>
+  </si>
+  <si>
+    <t>shell curtain</t>
+  </si>
+  <si>
+    <t>ThingDef+GM_Mer_ShellCurtain.description</t>
+  </si>
+  <si>
+    <t>GM_Mer_ShellCurtain.description</t>
+  </si>
+  <si>
+    <t>Divides rooms. A simple curtain made with elaborated shell-shaped textiles, doesn't slow people down but also doesn't retain heat.</t>
+  </si>
+  <si>
+    <t>ThingStyleDef+Ocean_Spear.overrideLabel</t>
+  </si>
+  <si>
+    <t>ThingStyleDef</t>
+  </si>
+  <si>
+    <t>Ocean_Spear.overrideLabel</t>
+  </si>
+  <si>
+    <t>heavy trident</t>
+  </si>
+  <si>
+    <t>ThingStyleDef+Ocean_Pila.overrideLabel</t>
+  </si>
+  <si>
+    <t>Ocean_Pila.overrideLabel</t>
+  </si>
+  <si>
+    <t>trident</t>
+  </si>
+  <si>
+    <t>ThingStyleDef+Ocean_Duster.overrideLabel</t>
+  </si>
+  <si>
+    <t>Ocean_Duster.overrideLabel</t>
+  </si>
+  <si>
+    <t>floaty duster</t>
+  </si>
+  <si>
+    <t>ThingStyleDef+Ocean_Jacket.overrideLabel</t>
+  </si>
+  <si>
+    <t>Ocean_Jacket.overrideLabel</t>
+  </si>
+  <si>
+    <t>leafy jacket</t>
+  </si>
+  <si>
+    <t>ThingStyleDef+Ocean_Bed.overrideLabel</t>
+  </si>
+  <si>
+    <t>Ocean_Bed.overrideLabel</t>
+  </si>
+  <si>
+    <t>hammock</t>
+  </si>
+  <si>
+    <t>ThingStyleDef+Ocean_FabricationBench.overrideLabel</t>
+  </si>
+  <si>
+    <t>Ocean_FabricationBench.overrideLabel</t>
+  </si>
+  <si>
+    <t>fabrication zone</t>
+  </si>
+  <si>
+    <t>OceanFineTile_Sandstone.description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해저 석판 (중형)</t>
+  </si>
+  <si>
+    <t>바닥을 장식하기 위한 해저 양식의 석재 부조입니다.</t>
+  </si>
+  <si>
+    <t>해저 석판 (대형)</t>
+  </si>
+  <si>
+    <t>해저</t>
+  </si>
+  <si>
+    <t>바닥을 장식하기 위한 해저 양식의 석재 부조입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멋진 해저 사암 바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멋진 해저 화강암 바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멋진 해저 석회암 바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멋진 해저 점판암 바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멋진 해저 대리석 바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해저 석재 바닥</t>
+  </si>
+  <si>
+    <t>해저 사암 바닥</t>
+  </si>
+  <si>
+    <t>해저 화강암 바닥</t>
+  </si>
+  <si>
+    <t>해저 석회암 바닥</t>
+  </si>
+  <si>
+    <t>해저 점판암 바닥</t>
+  </si>
+  <si>
+    <t>해저 대리석 바닥</t>
+  </si>
+  <si>
+    <t>원칙을 굽히지 않고 만든 정교한 해저 양식 석재 바닥으로, 경제적인 지위를 나타냅니다. 건설 속도가 느립니다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멋진 해저 바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멋진 태초의 해저 석회암 바닥</t>
+  </si>
+  <si>
+    <t>태초의 해저 석회암 바닥</t>
+  </si>
+  <si>
+    <t>해저 양식 양탄자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해저 양탄자 ({0})</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파도 아래 깊은 바다를 묘사한 부드러운 양탄자입니다. 안락하고 편안하며 보기에 좋지만 불에 타기 쉽고 청소하기 어렵습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파도 아래 깊은 바다를 묘사한 거칠게 다듬은 돌 바닥입니다. 예쁘진 않지만 도로나 보행로를 만들기에는 좋습니다. 판석은 해체해도 자재를 돌려받을 수 없습니다.</t>
+  </si>
+  <si>
+    <t>조개껍질 커튼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>조개껍질 형상으로 직조된 커튼입니다. 움직이는 데 걸리적거리지 않지만, 온도를 유지하는 기능 또한 없습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>무거운 삼지창</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼지창</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>깃털 먼지떨이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나뭇잎 조끼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해먹</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>제조 구역</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -108,7 +559,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -127,13 +578,24 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,9 +610,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -452,11 +915,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -505,7 +968,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -522,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -539,7 +1002,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -556,15 +1019,15 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -573,11 +1036,641 @@
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>